<commit_message>
update detail satuan sampah dan add fitur cancel setoran
</commit_message>
<xml_diff>
--- a/public/Daftar Limbah.xlsx
+++ b/public/Daftar Limbah.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>No</t>
   </si>
@@ -29,53 +29,13 @@
     <t>Harga</t>
   </si>
   <si>
-    <t>2023-08-09</t>
-  </si>
-  <si>
-    <t>Cairan</t>
-  </si>
-  <si>
-    <t>Cairan1</t>
-  </si>
-  <si>
-    <t>Cairan2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan3
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan4
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan5
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan6
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan7
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan8
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cairan9
-</t>
-  </si>
-  <si>
-    <t>2023-08-08</t>
-  </si>
-  <si>
-    <t>Cair</t>
-  </si>
-  <si>
-    <t>Padat</t>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>cair</t>
+  </si>
+  <si>
+    <t>padat</t>
   </si>
 </sst>
 </file>
@@ -415,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,147 +422,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>5000</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>